<commit_message>
added async, and cleaned folders
ready for run
</commit_message>
<xml_diff>
--- a/datasets/runable_problems/exam_questions.xlsx
+++ b/datasets/runable_problems/exam_questions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy Blumental\NLP\nlp-tau\datasets\runable_problems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\nlp\final_project\nlp-tau\datasets\runable_problems\hide\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5058F775-C865-4E76-A530-C2E168AA41EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{9AF1A329-B131-44DA-9EEC-75022146EE01}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="21690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,12 +550,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -919,19 +918,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92CA944-6086-4AB5-B8AE-A7AB2C54EF14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27.08984375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>100</v>
       </c>
@@ -939,7 +935,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -947,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -955,7 +951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -963,7 +959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -971,7 +967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -979,7 +975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -987,7 +983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -995,7 +991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1003,7 +999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1011,7 +1007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1019,7 +1015,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +1023,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1035,7 +1031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1043,7 +1039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1051,7 +1047,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1059,7 +1055,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1067,7 +1063,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1075,7 +1071,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1083,7 +1079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
@@ -1091,7 +1087,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1099,7 +1095,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1107,7 +1103,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
@@ -1115,7 +1111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -1123,7 +1119,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -1131,7 +1127,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="392" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1139,7 +1135,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
@@ -1147,7 +1143,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="378" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
@@ -1155,7 +1151,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -1163,7 +1159,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="406" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="392" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
@@ -1171,7 +1167,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="377" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="364" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -1179,7 +1175,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -1187,7 +1183,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>63</v>
       </c>
@@ -1195,7 +1191,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
@@ -1203,7 +1199,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
@@ -1211,7 +1207,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
@@ -1219,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
@@ -1227,7 +1223,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
@@ -1235,7 +1231,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1243,7 +1239,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1251,7 +1247,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>76</v>
       </c>
@@ -1259,7 +1255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -1267,7 +1263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1275,7 +1271,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="280" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1283,7 +1279,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -1291,7 +1287,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -1299,7 +1295,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="232" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="224" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -1307,7 +1303,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -1315,7 +1311,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -1323,7 +1319,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -1331,7 +1327,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>98</v>
       </c>

</xml_diff>